<commit_message>
update testcase create account
</commit_message>
<xml_diff>
--- a/data/DataInput/create Account.xlsx
+++ b/data/DataInput/create Account.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\kiemchungphanmem\code selenium\DataInput\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\phatrienphanmem\DataInput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0903C485-5611-4370-B922-F33DC6BA9A22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB17EC8A-4C7B-45E9-9266-ABB603A1264F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="149">
   <si>
     <t>ID</t>
   </si>
@@ -99,367 +99,400 @@
     <t>Đăng kí không thành công | Đữ liệu đầy đủ</t>
   </si>
   <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>ConfirmPassword</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>What is your favorite colors?</t>
+  </si>
+  <si>
+    <t>What is your father's nickname?</t>
+  </si>
+  <si>
+    <t>1testvip-123</t>
+  </si>
+  <si>
+    <t>1testvip-124</t>
+  </si>
+  <si>
+    <t>1testvip-125</t>
+  </si>
+  <si>
+    <t>1testvip-126</t>
+  </si>
+  <si>
+    <t>1testvip-127</t>
+  </si>
+  <si>
+    <t>1testvip-128</t>
+  </si>
+  <si>
+    <t>1testvip-129</t>
+  </si>
+  <si>
+    <t>1testvip-130</t>
+  </si>
+  <si>
+    <t>1testvip-131</t>
+  </si>
+  <si>
+    <t>1testvip-136</t>
+  </si>
+  <si>
+    <t>1testvip-137</t>
+  </si>
+  <si>
+    <t>1testvip-139</t>
+  </si>
+  <si>
+    <t>1testvip-141</t>
+  </si>
+  <si>
+    <t>1testvip-142</t>
+  </si>
+  <si>
+    <t>1testvip-143</t>
+  </si>
+  <si>
+    <t>1testvip-145</t>
+  </si>
+  <si>
+    <t>1testvip-146</t>
+  </si>
+  <si>
+    <t>testVip11@gmail.com</t>
+  </si>
+  <si>
+    <t>testVip12@gmail.com</t>
+  </si>
+  <si>
+    <t>testVip13@gmail.com</t>
+  </si>
+  <si>
+    <t>testVip14@gmail.com</t>
+  </si>
+  <si>
+    <t>testVip15@gmail.com</t>
+  </si>
+  <si>
+    <t>testVip16@gmail.com</t>
+  </si>
+  <si>
+    <t>testVip17@gmail.com</t>
+  </si>
+  <si>
+    <t>testVip18@gmail.com</t>
+  </si>
+  <si>
+    <t>testVip23@gmail.com</t>
+  </si>
+  <si>
+    <t>testVip22@gmail.com</t>
+  </si>
+  <si>
+    <t>testVip20@gmail.com</t>
+  </si>
+  <si>
+    <t>testVip19@gmail.com</t>
+  </si>
+  <si>
+    <t>testVip10@gmail.com</t>
+  </si>
+  <si>
+    <t>Red0</t>
+  </si>
+  <si>
+    <t>Red1</t>
+  </si>
+  <si>
+    <t>Red2</t>
+  </si>
+  <si>
+    <t>Red3</t>
+  </si>
+  <si>
+    <t>Red4</t>
+  </si>
+  <si>
+    <t>Red5</t>
+  </si>
+  <si>
+    <t>Red6</t>
+  </si>
+  <si>
+    <t>Red7</t>
+  </si>
+  <si>
+    <t>Red8</t>
+  </si>
+  <si>
+    <t>Red9</t>
+  </si>
+  <si>
+    <t>Red10</t>
+  </si>
+  <si>
+    <t>Red11</t>
+  </si>
+  <si>
+    <t>Red12</t>
+  </si>
+  <si>
+    <t>Red13</t>
+  </si>
+  <si>
+    <t>Red14</t>
+  </si>
+  <si>
+    <t>Red15</t>
+  </si>
+  <si>
+    <t>Red16</t>
+  </si>
+  <si>
+    <t>Red17</t>
+  </si>
+  <si>
+    <t>Red18</t>
+  </si>
+  <si>
+    <t>Red22</t>
+  </si>
+  <si>
+    <t>Red23</t>
+  </si>
+  <si>
+    <t>1testvip &amp;%#-132</t>
+  </si>
+  <si>
+    <t>1t133</t>
+  </si>
+  <si>
+    <t>Đăng kí thành công | Đăng ký với mật khẩu bao gồm chữ và số và ký tự đật biệt</t>
+  </si>
+  <si>
+    <t>Đăng kí thành công | Đăng ký với xác nhận mật khẩu có ký tự đặt biệt</t>
+  </si>
+  <si>
+    <t>p-138</t>
+  </si>
+  <si>
+    <t>Đăng kí thành công | Đăng ký với xác nhận mật khẩu bao gồm chữ và số và ký tự đặt biệt</t>
+  </si>
+  <si>
+    <t>1testvip-141eee</t>
+  </si>
+  <si>
+    <t>Red20---?&gt;&lt;%$</t>
+  </si>
+  <si>
+    <t>1tes!@#$%^&amp;*()_+tvip-136</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>testVip3@gmail.com</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>testVip4@gmail.com</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>testVip6asd---*&amp;^%$#@!------r@gmail.com</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>testVip7sdfdsfdsafsdfsdfdsafsadfsdafadsfjkljfkasdjflksdafjsladkjfkladsjfkadsjfkdsajfkjsdklfjasdkadsfsadfsaf242332dlfjfsdafasdaskdfjkladsjfklwjkerjweklrjwklerjqewkljrwklejrklwqejrlkwejrklqesdafadsfasdfsadwjrlkwjrklwqjrkljwerkjqewklrjqewkrsfsdfajqewlkrjlkwqjrfasdfjlqwjrlkwqejrlkewrewqrsdfsadfadsfadsf@gmail.com</t>
+  </si>
+  <si>
+    <t>testVip8@gmail.com</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>testVip9@gmail.com</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>testVip21@gmail.com</t>
+  </si>
+  <si>
+    <t>testVip24@gmail.com</t>
+  </si>
+  <si>
+    <t>testVip25@gmail.com</t>
+  </si>
+  <si>
+    <t>userName3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>userName5</t>
+  </si>
+  <si>
+    <t>userName7</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>userName9!@#$%^&amp;*()_+6sd------</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>userName10sdfdsfdsafsdfsdfdsafsadfsdafadsfjkljfkasdjflksdafjsladkjfkladsjfkadsjfkdsajfkjsdklfjasdkadsfsadfsaf242332dlfjfsdafasdaskdfjkladsjfklwjkerjweklrjwklerjqewkljrwklejrklwqejrlkwejrklqesdafadsfasdfsadwjrlkwjrklwqjrkljwerkjqewklrjqewkrsfsdfajqewlkrjlkwqjrfasdfjlqwjrlkwqejrlkewrewqrsdfsadfadsfadsf</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>userName12</t>
+  </si>
+  <si>
+    <t>userName13</t>
+  </si>
+  <si>
+    <t>userName15</t>
+  </si>
+  <si>
+    <t>userName16</t>
+  </si>
+  <si>
+    <t>userName17</t>
+  </si>
+  <si>
+    <t>userName18</t>
+  </si>
+  <si>
+    <t>userName19</t>
+  </si>
+  <si>
+    <t>userName20</t>
+  </si>
+  <si>
+    <t>userName21</t>
+  </si>
+  <si>
+    <t>userName11</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>userName22</t>
+  </si>
+  <si>
+    <t>userName23</t>
+  </si>
+  <si>
+    <t>userName24</t>
+  </si>
+  <si>
+    <t>userName25</t>
+  </si>
+  <si>
     <t>FullName</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>UserName</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>ConfirmPassword</t>
-  </si>
-  <si>
-    <t>Question</t>
-  </si>
-  <si>
-    <t>Answer</t>
-  </si>
-  <si>
-    <t>What is your favorite colors?</t>
-  </si>
-  <si>
-    <t>What is your father's nickname?</t>
-  </si>
-  <si>
-    <t>asd---------</t>
-  </si>
-  <si>
-    <t>1testvip-123</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FullName3asd--!@#$%^&amp;*()_-------</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FullName4sdfdsfdsafsdfsdfdsafsadfsdafadsfjkljfkasdjflksdafjsladkjfkladsjfkadsjfkdsajfkjsdklfjasdkadsfsadfsaf242332dlfjfsdafasdaskdfjkladsjfklwjkerjweklrjwklerjqewkljrwklejrklwqejrlkwejrklqesdafadsfasdfsadwjrlkwjrklwqjrkljwerkjqewklrjqewkrsfsdfajqewlkrjlkwqjrfasdfjlqwjrlkwqejrlkewrewqrsdfsadfadsfadsf</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FullName5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FullName7</t>
+  </si>
+  <si>
+    <t>FullName8</t>
+  </si>
+  <si>
+    <t>FullName9</t>
+  </si>
+  <si>
+    <t>FullName10</t>
+  </si>
+  <si>
+    <t>FullName11</t>
+  </si>
+  <si>
+    <t>FullName12</t>
+  </si>
+  <si>
+    <t>FullName13</t>
+  </si>
+  <si>
+    <t>FullName14</t>
+  </si>
+  <si>
+    <t>FullName15</t>
+  </si>
+  <si>
+    <t>FullName16</t>
+  </si>
+  <si>
+    <t>FullName17</t>
+  </si>
+  <si>
+    <t>FullName18</t>
+  </si>
+  <si>
+    <t>FullName19</t>
+  </si>
+  <si>
+    <t>FullName20</t>
+  </si>
+  <si>
+    <t>FullName21</t>
+  </si>
+  <si>
+    <t>FullName22</t>
+  </si>
+  <si>
+    <t>FullName23</t>
+  </si>
+  <si>
+    <t>FullName24</t>
+  </si>
+  <si>
+    <t>FullName25</t>
+  </si>
+  <si>
+    <t>userName4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>1testvip-124</t>
-  </si>
-  <si>
-    <t>testVip1@gmail.com</t>
-  </si>
-  <si>
-    <t>testVip0@gmail.com</t>
-  </si>
-  <si>
-    <t>1testvip-125</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>userName14</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FullName6</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>userName6</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>1testvip-126</t>
-  </si>
-  <si>
-    <t>1testvip-127</t>
-  </si>
-  <si>
-    <t>1testvip-128</t>
-  </si>
-  <si>
-    <t>1testvip-129</t>
-  </si>
-  <si>
-    <t>1testvip-130</t>
-  </si>
-  <si>
-    <t>1testvip-131</t>
-  </si>
-  <si>
-    <t>1testvip-136</t>
-  </si>
-  <si>
-    <t>1testvip-137</t>
-  </si>
-  <si>
-    <t>1testvip-139</t>
-  </si>
-  <si>
-    <t>1testvip-141</t>
-  </si>
-  <si>
-    <t>1testvip-142</t>
-  </si>
-  <si>
-    <t>1testvip-143</t>
-  </si>
-  <si>
-    <t>1testvip-145</t>
-  </si>
-  <si>
-    <t>1testvip-146</t>
-  </si>
-  <si>
-    <t>testVip2</t>
-  </si>
-  <si>
-    <t>testVip3</t>
-  </si>
-  <si>
-    <t>testVip4</t>
-  </si>
-  <si>
-    <t>testVip5</t>
-  </si>
-  <si>
-    <t>testVip6</t>
-  </si>
-  <si>
-    <t>testVip7</t>
-  </si>
-  <si>
-    <t>testVip8</t>
-  </si>
-  <si>
-    <t>testVip9</t>
-  </si>
-  <si>
-    <t>testVip10</t>
-  </si>
-  <si>
-    <t>testVip11</t>
-  </si>
-  <si>
-    <t>testVip12</t>
-  </si>
-  <si>
-    <t>testVip13</t>
-  </si>
-  <si>
-    <t>testVip14</t>
-  </si>
-  <si>
-    <t>testVip15</t>
-  </si>
-  <si>
-    <t>testVip16</t>
-  </si>
-  <si>
-    <t>testVip17</t>
-  </si>
-  <si>
-    <t>testVip18</t>
-  </si>
-  <si>
-    <t>testVip19</t>
-  </si>
-  <si>
-    <t>testVip20</t>
-  </si>
-  <si>
-    <t>testVip22</t>
-  </si>
-  <si>
-    <t>testVip23</t>
-  </si>
-  <si>
-    <t>testVip5@gmail.com</t>
-  </si>
-  <si>
-    <t>testVip6@gmail.com</t>
-  </si>
-  <si>
-    <t>testVip7@gmail.com</t>
-  </si>
-  <si>
-    <t>testVip8@gmail.com</t>
-  </si>
-  <si>
-    <t>testVip9@gmail.com</t>
-  </si>
-  <si>
-    <t>testVip11@gmail.com</t>
-  </si>
-  <si>
-    <t>testVip12@gmail.com</t>
-  </si>
-  <si>
-    <t>testVip13@gmail.com</t>
-  </si>
-  <si>
-    <t>testVip14@gmail.com</t>
-  </si>
-  <si>
-    <t>testVip15@gmail.com</t>
-  </si>
-  <si>
-    <t>testVip16@gmail.com</t>
-  </si>
-  <si>
-    <t>testVip17@gmail.com</t>
-  </si>
-  <si>
-    <t>testVip18@gmail.com</t>
-  </si>
-  <si>
-    <t>testVip23@gmail.com</t>
-  </si>
-  <si>
-    <t>testVip22@gmail.com</t>
-  </si>
-  <si>
-    <t>testVip20@gmail.com</t>
-  </si>
-  <si>
-    <t>testVip19@gmail.com</t>
-  </si>
-  <si>
-    <t>testVip10@gmail.com</t>
-  </si>
-  <si>
-    <t>vip0</t>
-  </si>
-  <si>
-    <t>vip1</t>
-  </si>
-  <si>
-    <t>vip2</t>
-  </si>
-  <si>
-    <t>vip3</t>
-  </si>
-  <si>
-    <t>vip4</t>
-  </si>
-  <si>
-    <t>vip8</t>
-  </si>
-  <si>
-    <t>vip9</t>
-  </si>
-  <si>
-    <t>vip10</t>
-  </si>
-  <si>
-    <t>vip11</t>
-  </si>
-  <si>
-    <t>vip12</t>
-  </si>
-  <si>
-    <t>vip13</t>
-  </si>
-  <si>
-    <t>vip14</t>
-  </si>
-  <si>
-    <t>vip15</t>
-  </si>
-  <si>
-    <t>vip16</t>
-  </si>
-  <si>
-    <t>vip17</t>
-  </si>
-  <si>
-    <t>vip18</t>
-  </si>
-  <si>
-    <t>vip19</t>
-  </si>
-  <si>
-    <t>vip20</t>
-  </si>
-  <si>
-    <t>vip22</t>
-  </si>
-  <si>
-    <t>vip23</t>
-  </si>
-  <si>
-    <t>Red0</t>
-  </si>
-  <si>
-    <t>Red1</t>
-  </si>
-  <si>
-    <t>Red2</t>
-  </si>
-  <si>
-    <t>Red3</t>
-  </si>
-  <si>
-    <t>Red4</t>
-  </si>
-  <si>
-    <t>Red5</t>
-  </si>
-  <si>
-    <t>Red6</t>
-  </si>
-  <si>
-    <t>Red7</t>
-  </si>
-  <si>
-    <t>Red8</t>
-  </si>
-  <si>
-    <t>Red9</t>
-  </si>
-  <si>
-    <t>Red10</t>
-  </si>
-  <si>
-    <t>Red11</t>
-  </si>
-  <si>
-    <t>Red12</t>
-  </si>
-  <si>
-    <t>Red13</t>
-  </si>
-  <si>
-    <t>Red14</t>
-  </si>
-  <si>
-    <t>Red15</t>
-  </si>
-  <si>
-    <t>Red16</t>
-  </si>
-  <si>
-    <t>Red17</t>
-  </si>
-  <si>
-    <t>Red18</t>
-  </si>
-  <si>
-    <t>Red22</t>
-  </si>
-  <si>
-    <t>Red23</t>
-  </si>
-  <si>
-    <t>testVip3asd---------@gmail.com</t>
-  </si>
-  <si>
-    <t>vip6sd------</t>
-  </si>
-  <si>
-    <t>1testvip &amp;%#-132</t>
-  </si>
-  <si>
-    <t>1t133</t>
-  </si>
-  <si>
-    <t>Đăng kí thành công | Đăng ký với mật khẩu bao gồm chữ và số và ký tự đật biệt</t>
-  </si>
-  <si>
-    <t>Đăng kí thành công | Đăng ký với xác nhận mật khẩu có ký tự đặt biệt</t>
-  </si>
-  <si>
-    <t>p-138</t>
-  </si>
-  <si>
-    <t>Đăng kí thành công | Đăng ký với xác nhận mật khẩu bao gồm chữ và số và ký tự đặt biệt</t>
-  </si>
-  <si>
-    <t>1testvip-141eee</t>
-  </si>
-  <si>
-    <t>Red20---?&gt;&lt;%$</t>
-  </si>
-  <si>
-    <t>sdfdsfdsafsdfsdfdsafsadfsdafadsfjkljfkasdjflksdafjsladkjfkladsjfkadsjfkdsajfkjsdklfjasdkadsfsadfsaf242332dlfjfsdafasdaskdfjkladsjfklwjkerjweklrjwklerjqewkljrwklejrklwqejrlkwejrklqesdafadsfasdfsadwjrlkwjrklwqjrkljwerkjqewklrjqewkrsfsdfajqewlkrjlkwqjrfasdfjlqwjrlkwqejrlkewrewqrsdfsadfadsfadsf</t>
-  </si>
-  <si>
-    <t>sdfdsfdsafsdfsdfdsafsadfsdafadsfjkljfkasdjflksdafjsladkjfkladsjfkadsjfkdsajfkjsdklfjasdkadsfsadfsaf242332dlfjfsdafasdaskdfjkladsjfklwjkerjweklrjwklerjqewkljrwklejrklwqejrlkwejrklqesdafadsfasdfsadwjrlkwjrklwqjrkljwerkjqewklrjqewkrsfsdfajqewlkrjlkwqjrfasdfjlqwjrlkwqejrlkewrewqrsdfsadfadsfadsf@gmail.com</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -467,34 +500,34 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="176" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
@@ -503,7 +536,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -584,25 +617,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -887,24 +916,24 @@
   <dimension ref="A1:Y91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="50.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="50.75" defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="43.6640625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="23.44140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="13.75" style="5" customWidth="1"/>
+    <col min="2" max="2" width="43.625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="24.625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="23.5" style="5" customWidth="1"/>
+    <col min="5" max="5" width="13.625" style="5" customWidth="1"/>
     <col min="6" max="6" width="25" style="5" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="17.375" style="5" customWidth="1"/>
     <col min="8" max="8" width="27" style="5" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" style="5" customWidth="1"/>
-    <col min="10" max="16384" width="50.77734375" style="5"/>
+    <col min="9" max="9" width="14.375" style="5" customWidth="1"/>
+    <col min="10" max="16384" width="50.75" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="49.95" customHeight="1" thickBot="1">
+    <row r="1" spans="1:25" ht="49.9" customHeight="1" thickBot="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -912,25 +941,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -949,7 +978,7 @@
       <c r="X1" s="3"/>
       <c r="Y1" s="3"/>
     </row>
-    <row r="2" spans="1:25" s="2" customFormat="1" ht="49.95" customHeight="1" thickBot="1">
+    <row r="2" spans="1:25" s="2" customFormat="1" ht="49.9" customHeight="1" thickBot="1">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -962,11 +991,11 @@
       <c r="F2" s="7"/>
       <c r="G2" s="1"/>
       <c r="H2" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I2" s="7"/>
     </row>
-    <row r="3" spans="1:25" s="2" customFormat="1" ht="49.95" customHeight="1" thickBot="1">
+    <row r="3" spans="1:25" s="2" customFormat="1" ht="49.9" customHeight="1" thickBot="1">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -979,40 +1008,40 @@
       <c r="F3" s="7"/>
       <c r="G3" s="1"/>
       <c r="H3" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I3" s="7"/>
     </row>
-    <row r="4" spans="1:25" s="2" customFormat="1" ht="49.95" customHeight="1" thickBot="1">
+    <row r="4" spans="1:25" s="2" customFormat="1" ht="49.9" customHeight="1" thickBot="1">
       <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>37</v>
+      <c r="C4" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" s="2" customFormat="1" ht="49.95" customHeight="1" thickBot="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" s="2" customFormat="1" ht="49.9" customHeight="1" thickBot="1">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1020,28 +1049,28 @@
         <v>7</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>93</v>
-      </c>
       <c r="F5" s="7" t="s">
-        <v>35</v>
+        <v>144</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" s="2" customFormat="1" ht="49.95" customHeight="1" thickBot="1">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" s="2" customFormat="1" ht="49.9" customHeight="1" thickBot="1">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1049,26 +1078,26 @@
         <v>5</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>53</v>
+        <v>123</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="7" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" s="2" customFormat="1" ht="49.95" customHeight="1" thickBot="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" s="2" customFormat="1" ht="49.9" customHeight="1" thickBot="1">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1076,28 +1105,28 @@
         <v>4</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>133</v>
+        <v>146</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>94</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>95</v>
+        <v>147</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>39</v>
+        <v>148</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" s="2" customFormat="1" ht="49.95" customHeight="1" thickBot="1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" s="2" customFormat="1" ht="49.9" customHeight="1" thickBot="1">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1105,28 +1134,28 @@
         <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>144</v>
+        <v>124</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>95</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" s="2" customFormat="1" ht="49.95" customHeight="1" thickBot="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" s="2" customFormat="1" ht="49.9" customHeight="1" thickBot="1">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1134,26 +1163,26 @@
         <v>9</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>74</v>
+        <v>125</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>96</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" s="2" customFormat="1" ht="49.95" customHeight="1" thickBot="1">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" s="2" customFormat="1" ht="49.9" customHeight="1" thickBot="1">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1161,28 +1190,28 @@
         <v>10</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>134</v>
+        <v>126</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>104</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" s="2" customFormat="1" ht="49.95" customHeight="1" thickBot="1">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" s="2" customFormat="1" ht="49.9" customHeight="1" thickBot="1">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -1190,28 +1219,28 @@
         <v>11</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>76</v>
+        <v>127</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>61</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>143</v>
+        <v>105</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" s="2" customFormat="1" ht="49.95" customHeight="1" thickBot="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" s="2" customFormat="1" ht="49.9" customHeight="1" thickBot="1">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -1219,26 +1248,26 @@
         <v>12</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>77</v>
+        <v>128</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>49</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" s="2" customFormat="1" ht="49.95" customHeight="1" thickBot="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" s="2" customFormat="1" ht="49.9" customHeight="1" thickBot="1">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -1246,28 +1275,28 @@
         <v>13</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>78</v>
+        <v>129</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>50</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>135</v>
+        <v>83</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>135</v>
+        <v>83</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" s="2" customFormat="1" ht="49.95" customHeight="1" thickBot="1">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" s="2" customFormat="1" ht="49.9" customHeight="1" thickBot="1">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -1275,57 +1304,57 @@
         <v>14</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>91</v>
+        <v>130</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>136</v>
+        <v>84</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>136</v>
+        <v>84</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" s="2" customFormat="1" ht="49.95" customHeight="1" thickBot="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" s="2" customFormat="1" ht="49.9" customHeight="1" thickBot="1">
       <c r="A15" s="4">
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>137</v>
+        <v>85</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>79</v>
+        <v>131</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>52</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>45</v>
+        <v>145</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>91</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" s="2" customFormat="1" ht="49.95" customHeight="1" thickBot="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" s="2" customFormat="1" ht="49.9" customHeight="1" thickBot="1">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -1333,28 +1362,28 @@
         <v>15</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>80</v>
+        <v>132</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>53</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="F16" s="13">
+        <v>108</v>
+      </c>
+      <c r="F16" s="11">
         <v>12345678</v>
       </c>
-      <c r="G16" s="13">
+      <c r="G16" s="11">
         <v>12345678</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" s="2" customFormat="1" ht="49.95" customHeight="1" thickBot="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="2" customFormat="1" ht="49.9" customHeight="1" thickBot="1">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -1362,55 +1391,55 @@
         <v>16</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>81</v>
+        <v>133</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>54</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G17" s="7"/>
       <c r="H17" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" s="2" customFormat="1" ht="49.95" customHeight="1" thickBot="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="2" customFormat="1" ht="49.9" customHeight="1" thickBot="1">
       <c r="A18" s="4">
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>138</v>
+        <v>86</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>82</v>
+        <v>134</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>55</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" s="2" customFormat="1" ht="49.95" customHeight="1" thickBot="1">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" s="2" customFormat="1" ht="49.9" customHeight="1" thickBot="1">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -1418,57 +1447,57 @@
         <v>17</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>83</v>
+        <v>135</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>56</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>139</v>
+        <v>87</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>139</v>
+        <v>87</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" s="2" customFormat="1" ht="49.95" customHeight="1" thickBot="1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="2" customFormat="1" ht="49.9" customHeight="1" thickBot="1">
       <c r="A20" s="4">
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>140</v>
+        <v>88</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>84</v>
+        <v>136</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>60</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" s="2" customFormat="1" ht="49.95" customHeight="1" thickBot="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="2" customFormat="1" ht="49.9" customHeight="1" thickBot="1">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -1476,28 +1505,28 @@
         <v>18</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>85</v>
+        <v>137</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="F21" s="12">
+        <v>113</v>
+      </c>
+      <c r="F21" s="10">
         <v>12345678</v>
       </c>
-      <c r="G21" s="12">
+      <c r="G21" s="10">
         <v>12345678</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" s="2" customFormat="1" ht="49.95" customHeight="1" thickBot="1">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="2" customFormat="1" ht="49.9" customHeight="1" thickBot="1">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -1505,28 +1534,28 @@
         <v>19</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>86</v>
+        <v>138</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>98</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>141</v>
+        <v>89</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" s="2" customFormat="1" ht="49.95" customHeight="1" thickBot="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" s="2" customFormat="1" ht="49.9" customHeight="1" thickBot="1">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -1534,26 +1563,26 @@
         <v>20</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>90</v>
+        <v>139</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>58</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I23" s="7"/>
     </row>
-    <row r="24" spans="1:9" s="2" customFormat="1" ht="49.95" customHeight="1" thickBot="1">
+    <row r="24" spans="1:9" s="2" customFormat="1" ht="49.9" customHeight="1" thickBot="1">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -1561,28 +1590,28 @@
         <v>21</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>89</v>
+        <v>140</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" s="2" customFormat="1" ht="49.95" customHeight="1" thickBot="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="2" customFormat="1" ht="49.9" customHeight="1" thickBot="1">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -1590,28 +1619,28 @@
         <v>22</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>88</v>
+        <v>141</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>99</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" s="2" customFormat="1" ht="49.95" customHeight="1" thickBot="1">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="2" customFormat="1" ht="49.9" customHeight="1" thickBot="1">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -1619,25 +1648,25 @@
         <v>23</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>87</v>
+        <v>142</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>100</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>132</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="2" customFormat="1"/>
@@ -1708,10 +1737,13 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D7" r:id="rId1" xr:uid="{52D737DF-4EB8-4BA0-AA1A-193E78D5DD0A}"/>
-    <hyperlink ref="D8" r:id="rId2" display="sdfdsfdsafsdfsdfdsafsadfsdafadsfjkljfkasdjflksdafjsladkjfkladsjfkadsjfkdsajfkjsdklfjasdkadsfsadfsaf242332dlfjfsdafasdaskdfjkladsjfklwjkerjweklrjwklerjqewkljrwklejrklwqejrlkwejrklqesdafadsfasdfsadwjrlkwjrklwqjrkljwerkjqewklrjqewkrsfsdfajqewlkrjlkwqjrfasdfjlqwjrlkwqejrlkewrewqrsdfsadfadsfadsf@gmail.com" xr:uid="{3EA3E5E1-E7B8-42AB-AA5A-E547889FC990}"/>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{77E79B8E-F5E1-4BD0-8191-D4A5F2667D7E}"/>
+    <hyperlink ref="E10" r:id="rId2" xr:uid="{E154218C-06F7-4956-B102-3BF338BEC477}"/>
+    <hyperlink ref="F15" r:id="rId3" xr:uid="{CB33689A-F810-4C1C-906C-28128505E391}"/>
+    <hyperlink ref="G15" r:id="rId4" xr:uid="{2B5F80E5-FD19-4D50-A1AB-D4B1DCB6935F}"/>
+    <hyperlink ref="D7" r:id="rId5" xr:uid="{E9F185B5-9A71-46C9-94D8-D2F494A7A445}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>